<commit_message>
Work on combining drop and pick with movement.
</commit_message>
<xml_diff>
--- a/tools/body-calculator.xlsx
+++ b/tools/body-calculator.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\codecamp\git.codecamp.edu\230620\screeps\screeps-project\tools\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\codecamp\git.codecamp.edu\230620\screeps\carver230620-sandbox\screeps-project\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>move</t>
   </si>
@@ -48,6 +48,9 @@
   </si>
   <si>
     <t>heal</t>
+  </si>
+  <si>
+    <t>attack</t>
   </si>
 </sst>
 </file>
@@ -365,10 +368,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E11"/>
+  <dimension ref="B1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -390,11 +393,11 @@
         <v>50</v>
       </c>
       <c r="D2">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E2">
         <f>C2*D2</f>
-        <v>250</v>
+        <v>400</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
@@ -405,7 +408,7 @@
         <v>0</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E7" si="0">C3*D3</f>
+        <f t="shared" ref="E3:E8" si="0">C3*D3</f>
         <v>0</v>
       </c>
     </row>
@@ -423,65 +426,80 @@
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>80</v>
+      </c>
+      <c r="D5">
         <v>3</v>
       </c>
-      <c r="C5">
-        <v>150</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
       <c r="E5">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" ref="E5" si="1">C5*D5</f>
+        <v>240</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C6">
-        <v>250</v>
+        <v>150</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6">
         <f t="shared" si="0"/>
-        <v>250</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C7">
-        <v>10</v>
+        <v>250</v>
       </c>
       <c r="D7">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D10">
-        <f>D2-SUM(D3:D7)</f>
-        <v>-6</v>
-      </c>
-      <c r="E10">
-        <f>SUM(E2:E7)</f>
-        <v>600</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <v>10</v>
+      </c>
+      <c r="D8">
+        <v>5</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
+      <c r="D11">
+        <f>D2-SUM(D3:D8)</f>
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <f>SUM(E2:E8)</f>
+        <v>690</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
         <v>6</v>
       </c>
-      <c r="D11">
-        <f>3*SUM(D2:D7)</f>
+      <c r="D12">
+        <f>3*SUM(D2:D8)</f>
         <v>48</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix for travelTo and body part for bad balance.
</commit_message>
<xml_diff>
--- a/tools/body-calculator.xlsx
+++ b/tools/body-calculator.xlsx
@@ -371,7 +371,7 @@
   <dimension ref="B1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -393,35 +393,41 @@
         <v>50</v>
       </c>
       <c r="D2">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E2">
         <f>C2*D2</f>
-        <v>400</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>1</v>
       </c>
+      <c r="C3">
+        <v>50</v>
+      </c>
       <c r="D3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E8" si="0">C3*D3</f>
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>2</v>
       </c>
+      <c r="C4">
+        <v>100</v>
+      </c>
       <c r="D4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
@@ -432,11 +438,11 @@
         <v>80</v>
       </c>
       <c r="D5">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E5">
         <f t="shared" ref="E5" si="1">C5*D5</f>
-        <v>240</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
@@ -477,21 +483,21 @@
         <v>10</v>
       </c>
       <c r="D8">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E8">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D11">
         <f>D2-SUM(D3:D8)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="E11">
         <f>SUM(E2:E8)</f>
-        <v>690</v>
+        <v>300</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
@@ -500,7 +506,7 @@
       </c>
       <c r="D12">
         <f>3*SUM(D2:D8)</f>
-        <v>48</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>